<commit_message>
20230330 update: update test case and test data.
</commit_message>
<xml_diff>
--- a/TestData/TestCase.xlsx
+++ b/TestData/TestCase.xlsx
@@ -1,29 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\test\codegen\output\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\codegen\OutResult\Cloud\NET.SDK\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAAA33DA-63E3-4A25-96B2-2A218C010662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3D9AD0C-6B08-4085-83D6-136989B7FC89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="6" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlcn.WorksheetConnection_Sheet1C5E13" hidden="1">Sheet1!$C$5:$E$13</definedName>
+    <definedName name="_xlcn.WorksheetConnection_Sheet1C5E131" hidden="1">Sheet1!$C$5:$E$13</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId4"/>
     <pivotCache cacheId="1" r:id="rId5"/>
+    <pivotCache cacheId="7" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -55,7 +56,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Range-d213b4da-b744-44db-ac10-bdbf77e88844" autoDelete="1">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_Sheet1C5E13"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_Sheet1C5E131"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -64,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="7">
   <si>
     <t>Id</t>
   </si>
@@ -91,19 +92,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -129,11 +123,11 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -152,39 +146,6 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Roy Wang" refreshedDate="41655.427479861108" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="8" xr:uid="{00000000-000A-0000-FFFF-FFFF01000000}">
-  <cacheSource type="worksheet">
-    <worksheetSource ref="C5:E13" sheet="Sheet1"/>
-  </cacheSource>
-  <cacheFields count="3">
-    <cacheField name="Id" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="2" count="2">
-        <n v="1"/>
-        <n v="2"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="Name" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2" maxValue="9" count="5">
-        <n v="2"/>
-        <n v="6"/>
-        <n v="4"/>
-        <n v="9"/>
-        <n v="8"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="Count" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="7"/>
-    </cacheField>
-  </cacheFields>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
-      <x14:pivotCacheDefinition/>
-    </ext>
-  </extLst>
-</pivotCacheDefinition>
-</file>
-
-<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="Roy Wang" refreshedDate="42264.442985995367" backgroundQuery="1" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{00000000-000A-0000-FFFF-FFFF27000000}">
   <cacheSource type="external" connectionId="1"/>
   <cacheFields count="3">
@@ -284,54 +245,91 @@
 </pivotCacheDefinition>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Cells" refreshedDate="44954.874811574075" createdVersion="5" refreshedVersion="8" minRefreshableVersion="3" recordCount="8" xr:uid="{00000000-000A-0000-FFFF-FFFF01000000}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="C5:E13" sheet="Sheet1"/>
+  </cacheSource>
+  <cacheFields count="3">
+    <cacheField name="Id" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="2" count="2">
+        <n v="1"/>
+        <n v="2"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Name" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2" maxValue="9" count="5">
+        <n v="2"/>
+        <n v="6"/>
+        <n v="4"/>
+        <n v="9"/>
+        <n v="8"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Count" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="7" count="3">
+        <n v="3"/>
+        <n v="7"/>
+        <n v="0"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="8">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="8">
   <r>
     <x v="0"/>
     <x v="0"/>
-    <n v="3"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="0"/>
     <x v="0"/>
-    <n v="3"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="1"/>
     <x v="1"/>
-    <n v="7"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="0"/>
     <x v="2"/>
-    <n v="3"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="1"/>
     <x v="3"/>
-    <n v="0"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="0"/>
     <x v="0"/>
-    <n v="3"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="0"/>
     <x v="4"/>
-    <n v="3"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="0"/>
     <x v="0"/>
-    <n v="7"/>
+    <x v="1"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:D9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable3" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:D10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisCol" showAll="0">
       <items count="3">
@@ -340,7 +338,7 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField axis="axisRow" showAll="0" measureFilter="1">
+    <pivotField axis="axisRow" showAll="0">
       <items count="6">
         <item x="0"/>
         <item x="2"/>
@@ -355,7 +353,7 @@
   <rowFields count="1">
     <field x="1"/>
   </rowFields>
-  <rowItems count="5">
+  <rowItems count="6">
     <i>
       <x/>
     </i>
@@ -367,6 +365,9 @@
     </i>
     <i>
       <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
     </i>
     <i t="grand">
       <x/>
@@ -390,21 +391,91 @@
     <dataField name="Sum of Count" fld="2" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <filters count="2">
-    <filter fld="0" type="captionGreaterThan" evalOrder="-1" id="4" stringValue1="0">
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D2E2DBAA-4DE7-4C0F-8B0C-C5F3597E2F3D}" name="PivotTable1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:D9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="3">
+    <pivotField axis="axisCol" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0">
+      <items count="4">
+        <item x="2"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="0"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Count" fld="2" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <filters count="1">
+    <filter fld="1" type="captionGreaterThan" evalOrder="-1" id="1" stringValue1="3">
       <autoFilter ref="A1">
         <filterColumn colId="0">
           <customFilters>
-            <customFilter operator="greaterThan" val="0"/>
-          </customFilters>
-        </filterColumn>
-      </autoFilter>
-    </filter>
-    <filter fld="1" type="valueGreaterThan" evalOrder="-1" id="3" iMeasureFld="0">
-      <autoFilter ref="A1">
-        <filterColumn colId="0">
-          <customFilters>
-            <customFilter operator="greaterThan" val="1"/>
+            <customFilter operator="greaterThan" val="3"/>
           </customFilters>
         </filterColumn>
       </autoFilter>
@@ -421,7 +492,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:D10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
@@ -782,13 +853,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C5:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6:G13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="5" spans="3:5">
+    <row r="5" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>0</v>
       </c>
@@ -799,7 +870,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="3:5">
+    <row r="6" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>1</v>
       </c>
@@ -810,7 +881,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="3:5">
+    <row r="7" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>1</v>
       </c>
@@ -821,7 +892,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="3:5">
+    <row r="8" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C8">
         <v>2</v>
       </c>
@@ -832,7 +903,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="3:5">
+    <row r="9" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C9">
         <v>1</v>
       </c>
@@ -843,7 +914,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="3:5">
+    <row r="10" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C10">
         <v>2</v>
       </c>
@@ -854,7 +925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="3:5">
+    <row r="11" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C11">
         <v>1</v>
       </c>
@@ -865,7 +936,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="3:5">
+    <row r="12" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C12">
         <v>1</v>
       </c>
@@ -876,7 +947,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="3:5">
+    <row r="13" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C13">
         <v>1</v>
       </c>
@@ -888,13 +959,12 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{32971FB3-F72B-46D5-A92A-581E7ADFF691}">
-          <x14:colorSeries rgb="FF376092"/>
+        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap" xr2:uid="{46DF9E0D-C88D-4997-BC4E-6E53B7ED24C1}">
+          <x14:colorSeries rgb="FF323232"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
           <x14:colorMarkers rgb="FFD00000"/>
@@ -905,35 +975,79 @@
           <x14:sparklines>
             <x14:sparkline>
               <xm:f>Sheet1!C6:E6</xm:f>
-              <xm:sqref>G6</xm:sqref>
+              <xm:sqref>H6</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
               <xm:f>Sheet1!C7:E7</xm:f>
-              <xm:sqref>G7</xm:sqref>
+              <xm:sqref>H7</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
               <xm:f>Sheet1!C8:E8</xm:f>
-              <xm:sqref>G8</xm:sqref>
+              <xm:sqref>H8</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
               <xm:f>Sheet1!C9:E9</xm:f>
-              <xm:sqref>G9</xm:sqref>
+              <xm:sqref>H9</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
               <xm:f>Sheet1!C10:E10</xm:f>
-              <xm:sqref>G10</xm:sqref>
+              <xm:sqref>H10</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
               <xm:f>Sheet1!C11:E11</xm:f>
-              <xm:sqref>G11</xm:sqref>
+              <xm:sqref>H11</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
               <xm:f>Sheet1!C12:E12</xm:f>
-              <xm:sqref>G12</xm:sqref>
+              <xm:sqref>H12</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
               <xm:f>Sheet1!C13:E13</xm:f>
-              <xm:sqref>G13</xm:sqref>
+              <xm:sqref>H13</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{7AB02ACF-6CA4-4BF7-963D-3CFB18FFCC18}">
+          <x14:colorSeries rgb="FF323232"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>Sheet1!E6:E6</xm:f>
+              <xm:sqref>I6</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!E7:E7</xm:f>
+              <xm:sqref>I7</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!E8:E8</xm:f>
+              <xm:sqref>I8</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!E9:E9</xm:f>
+              <xm:sqref>I9</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!E10:E10</xm:f>
+              <xm:sqref>I10</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!E11:E11</xm:f>
+              <xm:sqref>I11</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!E12:E12</xm:f>
+              <xm:sqref>I12</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!E13:E13</xm:f>
+              <xm:sqref>I13</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -945,31 +1059,31 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A3:D9"/>
+  <dimension ref="A3:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A5" sqref="A3:D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="2.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" customWidth="1"/>
     <col min="5" max="6" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B4">
@@ -982,76 +1096,200 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
         <v>2</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="3">
         <v>16</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1">
+      <c r="C5" s="3"/>
+      <c r="D5" s="3">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="1">
-        <v>3</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="3">
+      <c r="B6" s="3">
+        <v>3</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1">
+      <c r="B7" s="3"/>
+      <c r="C7" s="3">
         <v>7</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="3">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
         <v>8</v>
       </c>
-      <c r="B8" s="1">
-        <v>3</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="3" t="s">
+      <c r="B8" s="3">
+        <v>3</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>9</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B10" s="3">
         <v>22</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C10" s="3">
         <v>7</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D10" s="3">
         <v>29</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E07B6ADE-1516-46BE-B85B-A2DBCED674DE}">
+  <dimension ref="A3:D9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:D8"/>
+      <pivotSelection pane="bottomRight" showHeader="1" extendable="1" start="4" max="6" activeRow="8" click="1" r:id="rId1">
+        <pivotArea dataOnly="0" fieldPosition="0">
+          <references count="1">
+            <reference field="1" count="1">
+              <x v="4"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotSelection>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>3</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>6</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3">
+        <v>7</v>
+      </c>
+      <c r="D6" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>8</v>
+      </c>
+      <c r="B7" s="3">
+        <v>3</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>9</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3">
+        <v>0</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="3">
+        <v>6</v>
+      </c>
+      <c r="C9" s="3">
+        <v>7</v>
+      </c>
+      <c r="D9" s="3">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A3:D10"/>
   <sheetViews>
@@ -1059,24 +1297,24 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.125" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
     <col min="3" max="3" width="2" customWidth="1"/>
-    <col min="4" max="4" width="11.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B4">
@@ -1089,82 +1327,76 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
         <v>2</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5">
         <v>16</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1">
+      <c r="D5">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="1">
-        <v>3</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="3">
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1">
+      <c r="C7">
         <v>7</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
         <v>8</v>
       </c>
-      <c r="B8" s="1">
-        <v>3</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="3">
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
         <v>9</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1">
+      <c r="C9">
         <v>0</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10">
         <v>22</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10">
         <v>7</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10">
         <v>29</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>